<commit_message>
add more driving dimensions
</commit_message>
<xml_diff>
--- a/4-CAD/driving_dimensions.xlsx
+++ b/4-CAD/driving_dimensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bunny320\Desktop\sechs\4-CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB313FA-5044-4D76-888F-716F400B892C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FB7888-53E1-4AC6-A599-38788E1C7707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="705" windowWidth="22365" windowHeight="14490" xr2:uid="{6FBC4ECA-700F-497B-AC23-B469C74B2D94}"/>
+    <workbookView xWindow="3015" yWindow="705" windowWidth="22365" windowHeight="14490" xr2:uid="{6FBC4ECA-700F-497B-AC23-B469C74B2D94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>bearing_61807_outer</t>
   </si>
   <si>
     <t>bearing_61807_inner</t>
+  </si>
+  <si>
+    <t>bearing_61814_inner</t>
+  </si>
+  <si>
+    <t>bearing_61814_outer</t>
+  </si>
+  <si>
+    <t>M3_adjustable</t>
+  </si>
+  <si>
+    <t>bearing_61705_outer</t>
+  </si>
+  <si>
+    <t>bearing_61705_inner</t>
+  </si>
+  <si>
+    <t>bearing_606_outer</t>
+  </si>
+  <si>
+    <t>gearbox_42_outer</t>
+  </si>
+  <si>
+    <t>gearbox_35_outer</t>
   </si>
 </sst>
 </file>
@@ -392,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7A1EDD-2571-4C54-B2B0-5734EE712C9A}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,6 +444,70 @@
         <v>47.1</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>90.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>